<commit_message>
Update N-MOSFET transistor Update BOM file Update the PCB file with schematics Set Relay type and add link to buy it from AliExpress
</commit_message>
<xml_diff>
--- a/Project Outputs for DC_Pump_Soft_Starter/DC_Pump_Soft_Starter.xlsx
+++ b/Project Outputs for DC_Pump_Soft_Starter/DC_Pump_Soft_Starter.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Altium\DC_Soft_Starter\DC_Pump_Soft_Starter\Project Outputs for DC_Pump_Soft_Starter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Electronic Projects\DC_Soft_Starter\DC_Pump_Soft_Starter\Project Outputs for DC_Pump_Soft_Starter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{122663F3-FE30-4CD3-AFC5-BF7B15B3677B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B93A4C8F-D623-4F31-8741-72EBB0E3D31A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3810" yWindow="3810" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="53">
   <si>
     <t>Component List</t>
   </si>
@@ -39,16 +39,13 @@
     <t>Report Date</t>
   </si>
   <si>
-    <t>DC_Pump_Soft_Starter.BomDoc</t>
-  </si>
-  <si>
     <t>DC_Pump_Soft_Starter.PrjPcb</t>
   </si>
   <si>
     <t>None</t>
   </si>
   <si>
-    <t>22.6.2024 г.</t>
+    <t>2.7.2024 г.</t>
   </si>
   <si>
     <t>Description</t>
@@ -57,13 +54,16 @@
     <t>CAP ALUM 10UF 20% 50V THRU HOLE</t>
   </si>
   <si>
-    <t>STANDARD RECTIFIER 1000V SOD-123</t>
+    <t xml:space="preserve"> SOD-123 SMD</t>
   </si>
   <si>
     <t>TERM BLOCK HDR 2POS 90DEG 3.5MM</t>
   </si>
   <si>
-    <t>N-Channel 55V 49A (Tc) 94W (Tc) Through Hole TO-220AB</t>
+    <t>TRKM S-Z L 12VDC</t>
+  </si>
+  <si>
+    <t>N-Channel 100V 33A (Tc) 94W (Tc) Through Hole TO-220AB</t>
   </si>
   <si>
     <t>TH Resistor</t>
@@ -93,7 +93,10 @@
     <t>D1</t>
   </si>
   <si>
-    <t>J1, J2</t>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>J2</t>
   </si>
   <si>
     <t>K1</t>
@@ -105,7 +108,10 @@
     <t>R1</t>
   </si>
   <si>
-    <t>R2, R3</t>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>R3</t>
   </si>
   <si>
     <t>#Column Name Error:' Layer</t>
@@ -132,7 +138,7 @@
     <t>106RSS050M</t>
   </si>
   <si>
-    <t>1N4007</t>
+    <t>1N4148W</t>
   </si>
   <si>
     <t>0395021002</t>
@@ -144,7 +150,7 @@
     <t>Supplier 1</t>
   </si>
   <si>
-    <t>Digikey</t>
+    <t>DigiKey</t>
   </si>
   <si>
     <t>Supplier Part Number 1</t>
@@ -162,7 +168,19 @@
     <t>118-CHP0805AFX-1003ELFCT-ND</t>
   </si>
   <si>
-    <t>Price</t>
+    <t>price</t>
+  </si>
+  <si>
+    <t>0.31</t>
+  </si>
+  <si>
+    <t>0.01</t>
+  </si>
+  <si>
+    <t>0.58</t>
+  </si>
+  <si>
+    <t>0.06</t>
   </si>
 </sst>
 </file>
@@ -794,7 +812,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N39"/>
+  <dimension ref="A1:N41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
@@ -869,21 +887,21 @@
         <v>2</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="6" t="s">
         <v>3</v>
       </c>
       <c r="F4" s="24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G4" s="8"/>
       <c r="H4" s="6" t="s">
         <v>4</v>
       </c>
       <c r="I4" s="32" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
@@ -910,7 +928,7 @@
     <row r="6" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="25" t="s">
         <v>16</v>
@@ -922,22 +940,22 @@
         <v>20</v>
       </c>
       <c r="F6" s="25" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G6" s="25" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H6" s="25" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I6" s="25" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J6" s="25" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="K6" s="25" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
@@ -946,7 +964,7 @@
     <row r="7" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A7" s="15"/>
       <c r="B7" s="26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="28" t="s">
         <v>17</v>
@@ -959,19 +977,19 @@
       </c>
       <c r="F7" s="30"/>
       <c r="G7" s="18" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H7" s="18" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="I7" s="18" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J7" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="K7" s="21">
-        <v>0.2</v>
+        <v>44</v>
+      </c>
+      <c r="K7" s="21" t="s">
+        <v>49</v>
       </c>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
@@ -980,7 +998,7 @@
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="10"/>
       <c r="B8" s="27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="29"/>
       <c r="D8" s="16">
@@ -991,19 +1009,19 @@
       </c>
       <c r="F8" s="31"/>
       <c r="G8" s="19" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H8" s="19" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="I8" s="19" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J8" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="K8" s="22">
-        <v>0.14000000000000001</v>
+        <v>45</v>
+      </c>
+      <c r="K8" s="22" t="s">
+        <v>50</v>
       </c>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
@@ -1012,30 +1030,30 @@
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="15"/>
       <c r="B9" s="26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" s="28"/>
       <c r="D9" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E9" s="30" t="s">
         <v>23</v>
       </c>
       <c r="F9" s="30"/>
       <c r="G9" s="18" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H9" s="18" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="I9" s="18" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J9" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="K9" s="21">
-        <v>1.3</v>
+        <v>46</v>
+      </c>
+      <c r="K9" s="21" t="s">
+        <v>51</v>
       </c>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
@@ -1043,7 +1061,9 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="10"/>
-      <c r="B10" s="27"/>
+      <c r="B10" s="27" t="s">
+        <v>11</v>
+      </c>
       <c r="C10" s="29"/>
       <c r="D10" s="16">
         <v>1</v>
@@ -1052,11 +1072,21 @@
         <v>24</v>
       </c>
       <c r="F10" s="31"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="22"/>
+      <c r="G10" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="H10" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="I10" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="J10" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="K10" s="22" t="s">
+        <v>51</v>
+      </c>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
@@ -1064,7 +1094,7 @@
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="15"/>
       <c r="B11" s="26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" s="28"/>
       <c r="D11" s="17">
@@ -1086,7 +1116,7 @@
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="10"/>
       <c r="B12" s="27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" s="29"/>
       <c r="D12" s="16">
@@ -1108,86 +1138,110 @@
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="15"/>
       <c r="B13" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="28" t="s">
-        <v>18</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="C13" s="28"/>
       <c r="D13" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E13" s="30" t="s">
         <v>27</v>
       </c>
       <c r="F13" s="30"/>
-      <c r="G13" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="H13" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="I13" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="J13" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="K13" s="21">
-        <v>1.2</v>
-      </c>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
     </row>
-    <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="23"/>
-      <c r="K14" s="23"/>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="10"/>
+      <c r="B14" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="16">
+        <v>1</v>
+      </c>
+      <c r="E14" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="31"/>
+      <c r="G14" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="H14" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="I14" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="J14" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="K14" s="22" t="s">
+        <v>52</v>
+      </c>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
     </row>
-    <row r="15" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" s="15"/>
+      <c r="B15" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="17">
+        <v>1</v>
+      </c>
+      <c r="E15" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="30"/>
+      <c r="G15" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="H15" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="I15" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="J15" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="K15" s="21" t="s">
+        <v>52</v>
+      </c>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
+    <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="23"/>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -1554,6 +1608,38 @@
       <c r="L39" s="2"/>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>